<commit_message>
get data to do report
</commit_message>
<xml_diff>
--- a/prune_result.xlsx
+++ b/prune_result.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
   <si>
     <t>acc1</t>
   </si>
@@ -37,79 +37,34 @@
     <t>rem_trainable_param</t>
   </si>
   <si>
-    <t>50.0</t>
+    <t>69.14</t>
   </si>
   <si>
     <t>None</t>
   </si>
   <si>
+    <t>69.159996</t>
+  </si>
+  <si>
+    <t>4_2_1</t>
+  </si>
+  <si>
+    <t>0.0037</t>
+  </si>
+  <si>
+    <t>0.0044</t>
+  </si>
+  <si>
+    <t>68.976</t>
+  </si>
+  <si>
     <t>2_1_1</t>
   </si>
   <si>
-    <t>0.0100</t>
-  </si>
-  <si>
-    <t>0.0106</t>
-  </si>
-  <si>
-    <t>0.0098</t>
-  </si>
-  <si>
-    <t>0.0104</t>
-  </si>
-  <si>
-    <t>2_2_1</t>
-  </si>
-  <si>
-    <t>0.0096</t>
-  </si>
-  <si>
-    <t>0.0</t>
-  </si>
-  <si>
-    <t>0.0094</t>
-  </si>
-  <si>
-    <t>0.0097</t>
-  </si>
-  <si>
-    <t>5_2_1</t>
-  </si>
-  <si>
-    <t>0.0092</t>
-  </si>
-  <si>
-    <t>0.0095</t>
-  </si>
-  <si>
-    <t>3_1_1</t>
-  </si>
-  <si>
-    <t>0.0091</t>
-  </si>
-  <si>
-    <t>0.0089</t>
-  </si>
-  <si>
-    <t>0.0087</t>
-  </si>
-  <si>
-    <t>3_2_1</t>
-  </si>
-  <si>
-    <t>0.0085</t>
-  </si>
-  <si>
-    <t>0.0090</t>
-  </si>
-  <si>
-    <t>0.0084</t>
-  </si>
-  <si>
-    <t>0.0082</t>
-  </si>
-  <si>
-    <t>0.0083</t>
+    <t>0.0036</t>
+  </si>
+  <si>
+    <t>0.0058</t>
   </si>
 </sst>
 </file>
@@ -467,13 +422,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:N8"/>
+  <dimension ref="A1:D8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:14">
+    <row r="1" spans="1:4">
       <c r="B1" s="1">
         <v>0</v>
       </c>
@@ -483,38 +438,8 @@
       <c r="D1" s="1">
         <v>2</v>
       </c>
-      <c r="E1" s="1">
-        <v>3</v>
-      </c>
-      <c r="F1" s="1">
-        <v>4</v>
-      </c>
-      <c r="G1" s="1">
-        <v>5</v>
-      </c>
-      <c r="H1" s="1">
-        <v>6</v>
-      </c>
-      <c r="I1" s="1">
-        <v>7</v>
-      </c>
-      <c r="J1" s="1">
-        <v>8</v>
-      </c>
-      <c r="K1" s="1">
-        <v>9</v>
-      </c>
-      <c r="L1" s="1">
-        <v>10</v>
-      </c>
-      <c r="M1" s="1">
-        <v>11</v>
-      </c>
-      <c r="N1" s="1">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="2" spans="1:14">
+    </row>
+    <row r="2" spans="1:4">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
@@ -522,43 +447,13 @@
         <v>7</v>
       </c>
       <c r="C2" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="D2" t="s">
-        <v>7</v>
-      </c>
-      <c r="E2" t="s">
-        <v>7</v>
-      </c>
-      <c r="F2" t="s">
-        <v>16</v>
-      </c>
-      <c r="G2" t="s">
-        <v>7</v>
-      </c>
-      <c r="H2" t="s">
-        <v>16</v>
-      </c>
-      <c r="I2" t="s">
-        <v>16</v>
-      </c>
-      <c r="J2" t="s">
-        <v>16</v>
-      </c>
-      <c r="K2" t="s">
-        <v>16</v>
-      </c>
-      <c r="L2" t="s">
-        <v>16</v>
-      </c>
-      <c r="M2" t="s">
-        <v>16</v>
-      </c>
-      <c r="N2" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="3" spans="1:14">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4">
       <c r="A3" s="1" t="s">
         <v>1</v>
       </c>
@@ -566,40 +461,13 @@
         <v>8</v>
       </c>
       <c r="C3" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="D3" t="s">
-        <v>9</v>
-      </c>
-      <c r="E3" t="s">
         <v>14</v>
       </c>
-      <c r="F3" t="s">
-        <v>14</v>
-      </c>
-      <c r="G3" t="s">
-        <v>19</v>
-      </c>
-      <c r="H3" t="s">
-        <v>22</v>
-      </c>
-      <c r="I3" t="s">
-        <v>14</v>
-      </c>
-      <c r="J3" t="s">
-        <v>22</v>
-      </c>
-      <c r="K3" t="s">
-        <v>26</v>
-      </c>
-      <c r="L3" t="s">
-        <v>26</v>
-      </c>
-      <c r="M3" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="4" spans="1:14">
+    </row>
+    <row r="4" spans="1:4">
       <c r="A4" s="1" t="s">
         <v>2</v>
       </c>
@@ -607,40 +475,13 @@
         <v>0</v>
       </c>
       <c r="C4">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="D4">
-        <v>18</v>
-      </c>
-      <c r="E4">
-        <v>20</v>
-      </c>
-      <c r="F4">
-        <v>16</v>
-      </c>
-      <c r="G4">
-        <v>92</v>
-      </c>
-      <c r="H4">
-        <v>56</v>
-      </c>
-      <c r="I4">
-        <v>16</v>
-      </c>
-      <c r="J4">
-        <v>52</v>
-      </c>
-      <c r="K4">
-        <v>40</v>
-      </c>
-      <c r="L4">
-        <v>44</v>
-      </c>
-      <c r="M4">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="5" spans="1:14">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4">
       <c r="A5" s="1" t="s">
         <v>3</v>
       </c>
@@ -648,40 +489,13 @@
         <v>0</v>
       </c>
       <c r="C5" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="D5" t="s">
-        <v>12</v>
-      </c>
-      <c r="E5" t="s">
         <v>15</v>
       </c>
-      <c r="F5" t="s">
-        <v>17</v>
-      </c>
-      <c r="G5" t="s">
-        <v>20</v>
-      </c>
-      <c r="H5" t="s">
-        <v>23</v>
-      </c>
-      <c r="I5" t="s">
-        <v>24</v>
-      </c>
-      <c r="J5" t="s">
-        <v>25</v>
-      </c>
-      <c r="K5" t="s">
-        <v>27</v>
-      </c>
-      <c r="L5" t="s">
-        <v>29</v>
-      </c>
-      <c r="M5" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="6" spans="1:14">
+    </row>
+    <row r="6" spans="1:4">
       <c r="A6" s="1" t="s">
         <v>4</v>
       </c>
@@ -689,40 +503,13 @@
         <v>0</v>
       </c>
       <c r="C6" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="D6" t="s">
-        <v>13</v>
-      </c>
-      <c r="E6" t="s">
-        <v>11</v>
-      </c>
-      <c r="F6" t="s">
-        <v>18</v>
-      </c>
-      <c r="G6" t="s">
-        <v>21</v>
-      </c>
-      <c r="H6" t="s">
-        <v>15</v>
-      </c>
-      <c r="I6" t="s">
-        <v>24</v>
-      </c>
-      <c r="J6" t="s">
-        <v>21</v>
-      </c>
-      <c r="K6" t="s">
-        <v>28</v>
-      </c>
-      <c r="L6" t="s">
-        <v>23</v>
-      </c>
-      <c r="M6" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="7" spans="1:14">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4">
       <c r="A7" s="1" t="s">
         <v>5</v>
       </c>
@@ -730,40 +517,13 @@
         <v>11689512</v>
       </c>
       <c r="C7">
-        <v>11666432</v>
+        <v>11606532</v>
       </c>
       <c r="D7">
-        <v>11645660</v>
-      </c>
-      <c r="E7">
-        <v>11622580</v>
-      </c>
-      <c r="F7">
-        <v>11604116</v>
-      </c>
-      <c r="G7">
-        <v>10756060</v>
-      </c>
-      <c r="H7">
-        <v>10659180</v>
-      </c>
-      <c r="I7">
-        <v>10640716</v>
-      </c>
-      <c r="J7">
-        <v>10550756</v>
-      </c>
-      <c r="K7">
-        <v>10458516</v>
-      </c>
-      <c r="L7">
-        <v>10357052</v>
-      </c>
-      <c r="M7">
-        <v>10340896</v>
-      </c>
-    </row>
-    <row r="8" spans="1:14">
+        <v>11592684</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4">
       <c r="A8" s="1" t="s">
         <v>6</v>
       </c>
@@ -771,37 +531,10 @@
         <v>11689512</v>
       </c>
       <c r="C8">
-        <v>11666432</v>
+        <v>11606532</v>
       </c>
       <c r="D8">
-        <v>11645660</v>
-      </c>
-      <c r="E8">
-        <v>11622580</v>
-      </c>
-      <c r="F8">
-        <v>11604116</v>
-      </c>
-      <c r="G8">
-        <v>10756060</v>
-      </c>
-      <c r="H8">
-        <v>10659180</v>
-      </c>
-      <c r="I8">
-        <v>10640716</v>
-      </c>
-      <c r="J8">
-        <v>10550756</v>
-      </c>
-      <c r="K8">
-        <v>10458516</v>
-      </c>
-      <c r="L8">
-        <v>10357052</v>
-      </c>
-      <c r="M8">
-        <v>10340896</v>
+        <v>11592684</v>
       </c>
     </row>
   </sheetData>

</xml_diff>